<commit_message>
retoques api ruckus view
</commit_message>
<xml_diff>
--- a/media/excel.xlsx
+++ b/media/excel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="241">
   <si>
     <t xml:space="preserve">BUESCAP01</t>
   </si>
@@ -181,6 +181,12 @@
     <t xml:space="preserve">192.168.112.60</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:2B:16:D0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">132373006295</t>
+  </si>
+  <si>
     <t xml:space="preserve">CREW1</t>
   </si>
   <si>
@@ -193,12 +199,21 @@
     <t xml:space="preserve">CREW2</t>
   </si>
   <si>
+    <t xml:space="preserve">libre</t>
+  </si>
+  <si>
     <t xml:space="preserve">BUESCAP13</t>
   </si>
   <si>
     <t xml:space="preserve">192.168.112.62</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:2B:01:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">132373005947</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUDITORIO</t>
   </si>
   <si>
@@ -325,18 +340,27 @@
     <t xml:space="preserve">192.168.112.76</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7B:60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003491</t>
+  </si>
+  <si>
     <t xml:space="preserve">LA PAMPA 1</t>
   </si>
   <si>
-    <t xml:space="preserve">libre</t>
-  </si>
-  <si>
     <t xml:space="preserve">BUESCAP28</t>
   </si>
   <si>
     <t xml:space="preserve">192.168.112.77</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:46:D0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002766</t>
+  </si>
+  <si>
     <t xml:space="preserve">LA PAMPA 2</t>
   </si>
   <si>
@@ -346,6 +370,12 @@
     <t xml:space="preserve">192.168.112.78</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7B:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003496</t>
+  </si>
+  <si>
     <t xml:space="preserve">GOLDEN 1</t>
   </si>
   <si>
@@ -355,6 +385,12 @@
     <t xml:space="preserve">192.168.112.79</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:78:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003270</t>
+  </si>
+  <si>
     <t xml:space="preserve">GOLDEN 2</t>
   </si>
   <si>
@@ -364,6 +400,12 @@
     <t xml:space="preserve">192.168.112.80</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7B:B0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003479</t>
+  </si>
+  <si>
     <t xml:space="preserve">CATALINAS 1</t>
   </si>
   <si>
@@ -373,6 +415,12 @@
     <t xml:space="preserve">192.168.112.81</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7C:B0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003372</t>
+  </si>
+  <si>
     <t xml:space="preserve">CATALINAS 2</t>
   </si>
   <si>
@@ -382,6 +430,12 @@
     <t xml:space="preserve">192.168.112.82</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:47:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002655</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOYER CATALINAS</t>
   </si>
   <si>
@@ -391,6 +445,12 @@
     <t xml:space="preserve">192.168.112.83</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:3C:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002753</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOYER LIBERTADOR 1</t>
   </si>
   <si>
@@ -400,6 +460,12 @@
     <t xml:space="preserve">192.168.112.84</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:77:B0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003291</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOYER LIBERTADOR 2</t>
   </si>
   <si>
@@ -409,6 +475,12 @@
     <t xml:space="preserve">192.168.112.85</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7C:A0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003407</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOYER LIBERTADOR 3</t>
   </si>
   <si>
@@ -418,6 +490,12 @@
     <t xml:space="preserve">192.168.112.86</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:48:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002661</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOYER LIBERTADOR 4</t>
   </si>
   <si>
@@ -427,6 +505,12 @@
     <t xml:space="preserve">192.168.112.87</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7B:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003495</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALON LIBERTADOR 1</t>
   </si>
   <si>
@@ -436,6 +520,12 @@
     <t xml:space="preserve">192.168.112.88</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:3C:A0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002744</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALON LIBERTADOR 2</t>
   </si>
   <si>
@@ -445,6 +535,12 @@
     <t xml:space="preserve">192.168.112.89</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:45:C0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002607</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALON LIBERTADOR 3</t>
   </si>
   <si>
@@ -454,6 +550,12 @@
     <t xml:space="preserve">192.168.112.90</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:79:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003247</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALON LIBERTADOR 4</t>
   </si>
   <si>
@@ -463,6 +565,12 @@
     <t xml:space="preserve">192.168.112.91</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7B:D0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003765</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALON LIBERTADOR 5</t>
   </si>
   <si>
@@ -472,6 +580,12 @@
     <t xml:space="preserve">192.168.112.92</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:3C:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002754</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALON LIBERTADOR 6</t>
   </si>
   <si>
@@ -481,6 +595,12 @@
     <t xml:space="preserve">192.168.112.93</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:44:90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379002624</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOYER RETIRO 1</t>
   </si>
   <si>
@@ -490,6 +610,12 @@
     <t xml:space="preserve">192.168.112.94</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:7D:C0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003484</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOYER RETIRO 2</t>
   </si>
   <si>
@@ -499,6 +625,12 @@
     <t xml:space="preserve">192.168.112.95</t>
   </si>
   <si>
+    <t xml:space="preserve">3C:46:A1:25:77:A0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003300</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALON RETIRO 1</t>
   </si>
   <si>
@@ -506,6 +638,12 @@
   </si>
   <si>
     <t xml:space="preserve">192.168.112.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3C:46:A1:25:7E:80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122379003341</t>
   </si>
   <si>
     <t xml:space="preserve">SALON RETIRO 2</t>
@@ -708,10 +846,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -925,8 +1063,14 @@
       <c r="B11" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="C11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="E11" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>5</v>
@@ -934,27 +1078,33 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>5</v>
@@ -962,628 +1112,754 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>112</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>117</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>113</v>
+        <v>125</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>127</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>116</v>
+        <v>130</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>119</v>
+        <v>135</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>137</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>122</v>
+        <v>140</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>125</v>
+        <v>145</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>147</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>128</v>
+        <v>150</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>152</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>131</v>
+        <v>155</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>157</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>134</v>
+        <v>160</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>162</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>137</v>
+        <v>165</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>167</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>140</v>
+        <v>170</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>172</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>143</v>
+        <v>175</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>177</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>146</v>
+        <v>180</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>182</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>149</v>
+        <v>185</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>152</v>
+        <v>190</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>192</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>155</v>
+        <v>195</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>197</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>158</v>
+        <v>200</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>202</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>160</v>
+        <v>204</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>161</v>
+        <v>205</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>207</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>170</v>
+        <v>216</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>172</v>
+        <v>218</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>173</v>
+        <v>219</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>176</v>
+        <v>222</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>177</v>
+        <v>223</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>180</v>
+        <v>226</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>181</v>
+        <v>227</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>182</v>
+        <v>228</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>184</v>
+        <v>230</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>186</v>
+        <v>232</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>187</v>
+        <v>233</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>193</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>